<commit_message>
Changes done by Nanditha and Krishnan
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chiranjeev\Documents\Investment case study Cohort-3\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -17,12 +12,12 @@
     <sheet name="Table-3.1" sheetId="5" r:id="rId3"/>
     <sheet name="Table-5.1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
-  <extLst>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>C1</t>
   </si>
@@ -357,13 +352,19 @@
   </si>
   <si>
     <t>Sector-wise Investment Analysis</t>
+  </si>
+  <si>
+    <t>permalink</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -632,47 +633,50 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,7 +738,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -786,7 +790,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -980,47 +984,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="3"/>
     <col min="2" max="2" width="63.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="15"/>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+    <row r="2" spans="1:3" ht="9.75" customHeight="1">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="15"/>
     </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:3" ht="18" customHeight="1">
+      <c r="A3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
@@ -1031,43 +1035,51 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="17">
+        <v>66370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" customHeight="1">
       <c r="A6" s="5">
         <v>2</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17"/>
-    </row>
-    <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="16">
+        <v>66368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="36" customHeight="1">
       <c r="A7" s="5">
         <v>3</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31.5" customHeight="1">
       <c r="A8" s="5">
         <v>4</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45.75" customHeight="1">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -1076,10 +1088,10 @@
       </c>
       <c r="C9" s="17"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="B10" s="11"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="B11" s="11"/>
     </row>
   </sheetData>
@@ -1090,50 +1102,51 @@
   <conditionalFormatting sqref="A5:A9">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1">
+      <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="27"/>
+    </row>
+    <row r="2" spans="1:3" ht="23.25" customHeight="1">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+    </row>
+    <row r="3" spans="1:3" ht="24.75" customHeight="1">
+      <c r="A3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-    </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+    </row>
+    <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1144,7 +1157,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="21.75" customHeight="1">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -1153,7 +1166,7 @@
       </c>
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="21.75" customHeight="1">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -1162,7 +1175,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1171,7 +1184,7 @@
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="12">
         <v>4</v>
       </c>
@@ -1180,7 +1193,7 @@
       </c>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="59.25" customHeight="1">
       <c r="A9" s="12">
         <v>5</v>
       </c>
@@ -1197,8 +1210,8 @@
   <conditionalFormatting sqref="A5:A9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
@@ -1210,38 +1223,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="27"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+    </row>
+    <row r="3" spans="1:3" ht="23.25" customHeight="1">
+      <c r="A3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
@@ -1252,7 +1265,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="17.25">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -1261,7 +1274,7 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="17.25">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -1270,7 +1283,7 @@
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17.25">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -1287,8 +1300,8 @@
   <conditionalFormatting sqref="A4:A7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
@@ -1299,14 +1312,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="56.85546875" customWidth="1"/>
@@ -1315,43 +1328,43 @@
     <col min="5" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="30"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="B1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="19">
         <v>1</v>
       </c>
@@ -1362,7 +1375,7 @@
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="19">
         <v>2</v>
       </c>
@@ -1373,7 +1386,7 @@
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="19">
         <v>3</v>
       </c>
@@ -1384,7 +1397,7 @@
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="19">
         <v>4</v>
       </c>
@@ -1395,7 +1408,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="19">
         <v>5</v>
       </c>
@@ -1406,7 +1419,7 @@
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="19">
         <v>6</v>
       </c>
@@ -1417,7 +1430,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="19">
         <v>7</v>
       </c>
@@ -1428,7 +1441,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="19">
         <v>8</v>
       </c>
@@ -1439,7 +1452,7 @@
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="19">
         <v>9</v>
       </c>
@@ -1450,7 +1463,7 @@
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="30.75" thickBot="1">
       <c r="A14" s="19">
         <v>10</v>
       </c>
@@ -1469,17 +1482,17 @@
   <conditionalFormatting sqref="B5">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -1489,9 +1502,9 @@
   <conditionalFormatting sqref="A5:E14">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
@@ -1501,8 +1514,8 @@
   <conditionalFormatting sqref="A5:A14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFFFEF9C"/>
         <color rgb="FF63BE7B"/>
       </colorScale>

</xml_diff>

<commit_message>
21-01-19 , changes from Nanditha and Krishnan
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>C1</t>
   </si>
@@ -358,6 +358,30 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.298306
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.182024
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.180935
+</t>
+  </si>
+  <si>
+    <t>Venture</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -574,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -677,6 +701,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -984,7 +1011,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1120,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1166,7 +1193,9 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="37" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1">
       <c r="A6" s="12">
@@ -1175,7 +1204,9 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="37" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="12">
@@ -1184,16 +1215,20 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" s="12">
+        <v>2.1437840000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" s="12">
         <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="37" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1">
       <c r="A9" s="12">
@@ -1202,7 +1237,9 @@
       <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1228,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1274,7 +1311,9 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="17.25">
       <c r="A6" s="6">
@@ -1283,7 +1322,9 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="17.25">
       <c r="A7" s="6">
@@ -1292,7 +1333,9 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
29-01-2019 changes to add country wise DF
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Table-3.1" sheetId="5" r:id="rId3"/>
     <sheet name="Table-5.1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
   <si>
     <t>C1</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>India</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -598,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -669,6 +672,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -702,9 +708,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1022,7 +1026,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1033,23 +1037,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="10" t="s">
@@ -1070,7 +1074,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="17">
-        <v>66370</v>
+        <v>66368</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1">
@@ -1159,21 +1163,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1">
       <c r="A4" s="10" t="s">
@@ -1193,7 +1197,7 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="26" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1204,7 +1208,7 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="26" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1226,7 +1230,7 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="26" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1265,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1277,21 +1281,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="s">
@@ -1360,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1374,23 +1378,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="22" t="s">
@@ -1438,9 +1442,15 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="19">

</xml_diff>